<commit_message>
Feat 1562  && feat 1623 (#1642)
* happy linter
</commit_message>
<xml_diff>
--- a/libs/ui/src/lib/assets/templates/import-deals-template.xlsx
+++ b/libs/ui/src/lib/assets/templates/import-deals-template.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="sales v2" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Film Sales</t>
   </si>
@@ -150,6 +150,19 @@
     <t xml:space="preserve">Sale price 
 currency</t>
   </si>
+  <si>
+    <t xml:space="preserve">Catch up start date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catch up end date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multidiff (date1 ; &lt;date2&gt; ; …)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holdback
+(media, start date, end date)</t>
+  </si>
 </sst>
 </file>
 
@@ -181,13 +194,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="18"/>
       <name val="Arial"/>
@@ -207,6 +213,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -307,15 +320,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,15 +332,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -344,6 +353,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -424,150 +437,172 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1048576"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11:Q35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="11:54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="26.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="28.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="15" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="27.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="6" t="s">
+      <c r="N8" s="4"/>
+      <c r="O8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="8" t="s">
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-    </row>
-    <row r="10" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="P9" s="7"/>
+      <c r="Q9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="N10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="O10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="P10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="10" t="s">
+      <c r="Q10" s="9" t="s">
         <v>27</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="U10" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -578,42 +613,49 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-  </mergeCells>
-  <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L9" type="list">
-      <formula1>#réf !!$B$2:$B$256</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M9:N9" type="list">
-      <formula1>#réf !!$A$2:$A$21</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O9:Q9" type="list">
-      <formula1>#réf !!$C$2:$C$83</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>